<commit_message>
added graphs titles, added used maps
</commit_message>
<xml_diff>
--- a/results/building-2f.xlsx
+++ b/results/building-2f.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="building-signs-2t" sheetId="1" r:id="rId1"/>
@@ -622,6 +622,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="cs-CZ"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0"/>
+              <a:t>Time to leave building (2 width doors)</a:t>
+            </a:r>
+            <a:endParaRPr lang="cs-CZ" sz="1600" b="1" i="0" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1009,6 +1028,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="cs-CZ"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0"/>
+              <a:t>Survival rate (2 width doors</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="cs-CZ" sz="1800" b="1" i="0" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2080,6 +2122,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="cs-CZ"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Survival rate exit-only (4 width vs 2 width doors)</a:t>
+            </a:r>
+            <a:endParaRPr lang="cs-CZ" sz="1800" b="1" i="0" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2368,6 +2429,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="cs-CZ"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Survival rate no-signs (4 width vs 2 width doors)</a:t>
+            </a:r>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2656,6 +2736,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="cs-CZ"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Survival rate signs (4 width vs 2 width doors)</a:t>
+            </a:r>
+            <a:endParaRPr lang="cs-CZ" sz="1800" b="1" i="0" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -14076,8 +14175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14438,8 +14537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>